<commit_message>
Bug fixes for Nback and added biopac recording for Pinel
</commit_message>
<xml_diff>
--- a/fMRI Tasks/WASABI Task-T1/N-back-2.xlsx
+++ b/fMRI Tasks/WASABI Task-T1/N-back-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msun\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\WASABI Task-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12A06DD-09A0-4719-A8B8-28E5B5C9E777}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF46FA1-D8D3-4706-8678-72FE95E091D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32070" yWindow="-23880" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="13">
   <si>
     <t>location</t>
   </si>
@@ -425,7 +425,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -490,8 +492,8 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,8 +535,8 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
-        <v>11</v>
+      <c r="C12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,8 +562,8 @@
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" t="s">
-        <v>11</v>
+      <c r="C15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,8 +621,8 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" t="s">
-        <v>11</v>
+      <c r="C22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,8 +648,8 @@
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
-        <v>11</v>
+      <c r="C25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,8 +699,8 @@
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" t="s">
-        <v>11</v>
+      <c r="C31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,8 +726,8 @@
       <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="C34" t="s">
-        <v>11</v>
+      <c r="C34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,8 +777,8 @@
       <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" t="s">
-        <v>11</v>
+      <c r="C40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,8 +804,8 @@
       <c r="B43" t="s">
         <v>4</v>
       </c>
-      <c r="C43" t="s">
-        <v>11</v>
+      <c r="C43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -861,8 +863,8 @@
       <c r="B50" t="s">
         <v>7</v>
       </c>
-      <c r="C50" t="s">
-        <v>11</v>
+      <c r="C50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,8 +890,8 @@
       <c r="B53" t="s">
         <v>6</v>
       </c>
-      <c r="C53" t="s">
-        <v>11</v>
+      <c r="C53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -931,8 +933,8 @@
       <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C58" t="s">
-        <v>11</v>
+      <c r="C58">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,8 +1008,8 @@
       <c r="B67" t="s">
         <v>10</v>
       </c>
-      <c r="C67" t="s">
-        <v>11</v>
+      <c r="C67">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1049,8 +1051,8 @@
       <c r="B72" t="s">
         <v>6</v>
       </c>
-      <c r="C72" t="s">
-        <v>11</v>
+      <c r="C72">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1076,8 +1078,8 @@
       <c r="B75" t="s">
         <v>7</v>
       </c>
-      <c r="C75" t="s">
-        <v>11</v>
+      <c r="C75">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,8 +1137,8 @@
       <c r="B82" t="s">
         <v>4</v>
       </c>
-      <c r="C82" t="s">
-        <v>11</v>
+      <c r="C82">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,8 +1164,8 @@
       <c r="B85" t="s">
         <v>5</v>
       </c>
-      <c r="C85" t="s">
-        <v>11</v>
+      <c r="C85">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1213,8 +1215,8 @@
       <c r="B91" t="s">
         <v>7</v>
       </c>
-      <c r="C91" t="s">
-        <v>11</v>
+      <c r="C91">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,8 +1242,8 @@
       <c r="B94" t="s">
         <v>7</v>
       </c>
-      <c r="C94" t="s">
-        <v>11</v>
+      <c r="C94">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,8 +1293,8 @@
       <c r="B100" t="s">
         <v>5</v>
       </c>
-      <c r="C100" t="s">
-        <v>11</v>
+      <c r="C100">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1318,8 +1320,8 @@
       <c r="B103" t="s">
         <v>4</v>
       </c>
-      <c r="C103" t="s">
-        <v>11</v>
+      <c r="C103">
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1377,8 +1379,8 @@
       <c r="B110" t="s">
         <v>7</v>
       </c>
-      <c r="C110" t="s">
-        <v>11</v>
+      <c r="C110">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,8 +1406,8 @@
       <c r="B113" t="s">
         <v>6</v>
       </c>
-      <c r="C113" t="s">
-        <v>11</v>
+      <c r="C113">
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1447,8 +1449,8 @@
       <c r="B118" t="s">
         <v>10</v>
       </c>
-      <c r="C118" t="s">
-        <v>11</v>
+      <c r="C118">
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>